<commit_message>
Added Multiplexer/6 Flame Sensor Code, updated connections.xlsx
</commit_message>
<xml_diff>
--- a/arduino/ffrobot/connections.xlsx
+++ b/arduino/ffrobot/connections.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
   <si>
     <t>Analog Pins</t>
   </si>
@@ -181,13 +181,109 @@
   </si>
   <si>
     <t>Gyroscope</t>
+  </si>
+  <si>
+    <t>Multiplexer Select 1</t>
+  </si>
+  <si>
+    <t>Multiplexer Select 2</t>
+  </si>
+  <si>
+    <t>Multiplexer Select 3</t>
+  </si>
+  <si>
+    <t>4051 Pinout</t>
+  </si>
+  <si>
+    <t>CH 4 I/O</t>
+  </si>
+  <si>
+    <t>CH 6 I/O</t>
+  </si>
+  <si>
+    <t>COM O/I</t>
+  </si>
+  <si>
+    <t>CH 7 I/O</t>
+  </si>
+  <si>
+    <t>CH 5 I/O</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SS</t>
+    </r>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>CH 2 I/O</t>
+  </si>
+  <si>
+    <t>CH 1 I/O</t>
+  </si>
+  <si>
+    <t>CH 0 I/O</t>
+  </si>
+  <si>
+    <t>CH 3 I/O</t>
+  </si>
+  <si>
+    <t>INH</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DD</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,13 +299,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -224,9 +333,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -534,7 +647,7 @@
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +658,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -553,7 +666,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -561,7 +674,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -569,7 +682,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -577,7 +690,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -585,12 +698,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -601,17 +714,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -622,7 +735,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -632,8 +745,11 @@
       <c r="C13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="H13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -643,65 +759,170 @@
       <c r="C14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>16</v>
+      </c>
+      <c r="J14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="G15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="3">
+        <v>2</v>
+      </c>
+      <c r="I15" s="2">
+        <v>15</v>
+      </c>
+      <c r="J15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>10</v>
       </c>
       <c r="B16" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="3">
+        <v>3</v>
+      </c>
+      <c r="I16" s="2">
+        <v>14</v>
+      </c>
+      <c r="J16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>7</v>
       </c>
       <c r="B17" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="G17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="3">
+        <v>4</v>
+      </c>
+      <c r="I17" s="2">
+        <v>13</v>
+      </c>
+      <c r="J17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="G18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="3">
+        <v>5</v>
+      </c>
+      <c r="I18" s="2">
+        <v>12</v>
+      </c>
+      <c r="J18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="G19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="3">
+        <v>6</v>
+      </c>
+      <c r="I19" s="2">
+        <v>11</v>
+      </c>
+      <c r="J19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="G20" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="3">
+        <v>7</v>
+      </c>
+      <c r="I20" s="2">
+        <v>10</v>
+      </c>
+      <c r="J20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="3">
+        <v>8</v>
+      </c>
+      <c r="I21" s="2">
+        <v>9</v>
+      </c>
+      <c r="J21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -712,37 +933,37 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Partial reflection code added
</commit_message>
<xml_diff>
--- a/arduino/ffrobot/connections.xlsx
+++ b/arduino/ffrobot/connections.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="93">
   <si>
     <t>Analog Pins</t>
   </si>
@@ -277,6 +277,60 @@
       </rPr>
       <t>DD</t>
     </r>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>s3</t>
+  </si>
+  <si>
+    <t>s4</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>s5</t>
+  </si>
+  <si>
+    <t>s6</t>
+  </si>
+  <si>
+    <t>s7</t>
+  </si>
+  <si>
+    <t>com</t>
+  </si>
+  <si>
+    <t>inh</t>
+  </si>
+  <si>
+    <t>vee</t>
+  </si>
+  <si>
+    <t>vss</t>
+  </si>
+  <si>
+    <t>s0</t>
+  </si>
+  <si>
+    <t>vdd</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -307,7 +361,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +371,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,13 +393,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -659,20 +720,22 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>45</v>
       </c>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
@@ -773,12 +836,13 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="C15" s="4"/>
       <c r="G15" t="s">
         <v>60</v>
       </c>
@@ -793,12 +857,13 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="C16" s="4"/>
       <c r="G16" t="s">
         <v>61</v>
       </c>
@@ -813,12 +878,13 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="C17" s="4"/>
       <c r="G17" t="s">
         <v>62</v>
       </c>
@@ -833,12 +899,13 @@
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>51</v>
       </c>
+      <c r="C18" s="4"/>
       <c r="G18" t="s">
         <v>63</v>
       </c>
@@ -1022,6 +1089,190 @@
     <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="59" spans="6:15">
+      <c r="I59" t="s">
+        <v>87</v>
+      </c>
+      <c r="J59" t="s">
+        <v>80</v>
+      </c>
+      <c r="K59" t="s">
+        <v>80</v>
+      </c>
+      <c r="L59" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="6:15">
+      <c r="I60" t="s">
+        <v>86</v>
+      </c>
+      <c r="J60" t="s">
+        <v>80</v>
+      </c>
+      <c r="K60" t="s">
+        <v>80</v>
+      </c>
+      <c r="L60" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="6:15">
+      <c r="I61" t="s">
+        <v>85</v>
+      </c>
+      <c r="J61" t="s">
+        <v>80</v>
+      </c>
+      <c r="K61" t="s">
+        <v>80</v>
+      </c>
+      <c r="L61" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="6:15">
+      <c r="I62" t="s">
+        <v>81</v>
+      </c>
+      <c r="J62" t="s">
+        <v>80</v>
+      </c>
+      <c r="K62" t="s">
+        <v>80</v>
+      </c>
+      <c r="L62" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="6:15">
+      <c r="F63" t="s">
+        <v>83</v>
+      </c>
+      <c r="G63" t="s">
+        <v>79</v>
+      </c>
+      <c r="H63">
+        <v>5</v>
+      </c>
+      <c r="I63" t="s">
+        <v>83</v>
+      </c>
+      <c r="J63" t="s">
+        <v>80</v>
+      </c>
+      <c r="K63" t="s">
+        <v>80</v>
+      </c>
+      <c r="L63" t="s">
+        <v>88</v>
+      </c>
+      <c r="M63" t="s">
+        <v>77</v>
+      </c>
+      <c r="N63" t="s">
+        <v>79</v>
+      </c>
+      <c r="O63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="6:15">
+      <c r="F64" t="s">
+        <v>82</v>
+      </c>
+      <c r="G64" t="s">
+        <v>79</v>
+      </c>
+      <c r="H64">
+        <v>5</v>
+      </c>
+      <c r="I64" t="s">
+        <v>84</v>
+      </c>
+      <c r="J64" t="s">
+        <v>80</v>
+      </c>
+      <c r="K64" t="s">
+        <v>80</v>
+      </c>
+      <c r="L64" t="s">
+        <v>75</v>
+      </c>
+      <c r="M64" t="s">
+        <v>76</v>
+      </c>
+      <c r="N64" t="s">
+        <v>79</v>
+      </c>
+      <c r="O64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="6:15">
+      <c r="F65" t="s">
+        <v>81</v>
+      </c>
+      <c r="G65" t="s">
+        <v>79</v>
+      </c>
+      <c r="H65">
+        <v>5</v>
+      </c>
+      <c r="I65" t="s">
+        <v>82</v>
+      </c>
+      <c r="J65" t="s">
+        <v>80</v>
+      </c>
+      <c r="K65" t="s">
+        <v>80</v>
+      </c>
+      <c r="L65" t="s">
+        <v>76</v>
+      </c>
+      <c r="M65" t="s">
+        <v>75</v>
+      </c>
+      <c r="N65" t="s">
+        <v>79</v>
+      </c>
+      <c r="O65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="6:15">
+      <c r="F66" t="s">
+        <v>78</v>
+      </c>
+      <c r="G66" t="s">
+        <v>79</v>
+      </c>
+      <c r="H66">
+        <v>5</v>
+      </c>
+      <c r="I66" t="s">
+        <v>78</v>
+      </c>
+      <c r="J66" t="s">
+        <v>80</v>
+      </c>
+      <c r="K66" t="s">
+        <v>80</v>
+      </c>
+      <c r="L66" t="s">
+        <v>89</v>
+      </c>
+      <c r="M66" t="s">
+        <v>88</v>
+      </c>
+      <c r="N66" t="s">
+        <v>79</v>
+      </c>
+      <c r="O66">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Robot, finalized connections
</commit_message>
<xml_diff>
--- a/arduino/ffrobot/connections.xlsx
+++ b/arduino/ffrobot/connections.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19155" windowHeight="6975"/>
+    <workbookView xWindow="120" yWindow="80" windowWidth="19160" windowHeight="6980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
   <si>
     <t>Analog Pins</t>
   </si>
@@ -332,12 +337,15 @@
   <si>
     <t>reflector sensor</t>
   </si>
+  <si>
+    <t>spike relay</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -701,18 +709,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -947,6 +955,9 @@
       <c r="A20" t="s">
         <v>21</v>
       </c>
+      <c r="B20" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="G20" t="s">
         <v>63</v>
       </c>
@@ -1284,30 +1295,44 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First stage of intelligent search finished. all external functions are functioning (except gyro). all robot components functioning
</commit_message>
<xml_diff>
--- a/arduino/ffrobot/connections.xlsx
+++ b/arduino/ffrobot/connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="80" windowWidth="19160" windowHeight="6980"/>
+    <workbookView xWindow="120" yWindow="80" windowWidth="22480" windowHeight="20400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,7 +713,7 @@
   <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Gyroscope with internal timer overflow interrupt in place. still figuring out why it is not working right
</commit_message>
<xml_diff>
--- a/arduino/ffrobot/connections.xlsx
+++ b/arduino/ffrobot/connections.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="119">
   <si>
     <t>Analog Pins</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>Connection</t>
-  </si>
-  <si>
-    <t>front US sensor</t>
   </si>
   <si>
     <t>left us sensor</t>
@@ -340,12 +337,90 @@
   <si>
     <t>spike relay</t>
   </si>
+  <si>
+    <t>front us sensor</t>
+  </si>
+  <si>
+    <t>selectApin</t>
+  </si>
+  <si>
+    <t>selectBpin</t>
+  </si>
+  <si>
+    <t>selectCpin</t>
+  </si>
+  <si>
+    <t>leftSpeedPin</t>
+  </si>
+  <si>
+    <t>rightSpeedPin</t>
+  </si>
+  <si>
+    <t>leftDirPin</t>
+  </si>
+  <si>
+    <t>rightDirPin</t>
+  </si>
+  <si>
+    <t>reflectPin</t>
+  </si>
+  <si>
+    <t>fanPin</t>
+  </si>
+  <si>
+    <t>flameFLpin</t>
+  </si>
+  <si>
+    <t>flameFCpin</t>
+  </si>
+  <si>
+    <t>flameFRpin</t>
+  </si>
+  <si>
+    <t>flameBRpin</t>
+  </si>
+  <si>
+    <t>flameBCpin</t>
+  </si>
+  <si>
+    <t>flameBLpin</t>
+  </si>
+  <si>
+    <t>front left flame sensor</t>
+  </si>
+  <si>
+    <t>front center flame sensor</t>
+  </si>
+  <si>
+    <t>front right flame sensor</t>
+  </si>
+  <si>
+    <t>back right flame sensor</t>
+  </si>
+  <si>
+    <t>back center flame sensor</t>
+  </si>
+  <si>
+    <t>back left flame sensor</t>
+  </si>
+  <si>
+    <t>encoderPinL</t>
+  </si>
+  <si>
+    <t>encoderPinR</t>
+  </si>
+  <si>
+    <t>multiPin</t>
+  </si>
+  <si>
+    <t>gyroPin</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,8 +443,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,12 +479,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -404,8 +489,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -415,9 +520,29 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="21">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -713,7 +838,7 @@
   <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -723,7 +848,7 @@
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,54 +856,64 @@
         <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:10">
+        <v>43</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:10">
+        <v>44</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -786,56 +921,65 @@
         <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
       <c r="H13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>107</v>
       </c>
       <c r="G14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
@@ -844,19 +988,21 @@
         <v>16</v>
       </c>
       <c r="J14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H15" s="3">
         <v>2</v>
@@ -865,19 +1011,24 @@
         <v>15</v>
       </c>
       <c r="J15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>67</v>
+      </c>
+      <c r="K15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="G16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H16" s="3">
         <v>3</v>
@@ -886,19 +1037,24 @@
         <v>14</v>
       </c>
       <c r="J16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>68</v>
+      </c>
+      <c r="K16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="4"/>
+        <v>49</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="G17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H17" s="3">
         <v>4</v>
@@ -907,19 +1063,27 @@
         <v>13</v>
       </c>
       <c r="J17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>69</v>
+      </c>
+      <c r="K17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="G18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H18" s="3">
         <v>5</v>
@@ -928,18 +1092,24 @@
         <v>12</v>
       </c>
       <c r="J18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>70</v>
+      </c>
+      <c r="K18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="G19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H19" s="3">
         <v>6</v>
@@ -948,18 +1118,21 @@
         <v>11</v>
       </c>
       <c r="J19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>93</v>
+      <c r="B20" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H20" s="3">
         <v>7</v>
@@ -968,18 +1141,16 @@
         <v>10</v>
       </c>
       <c r="J20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
-        <v>54</v>
-      </c>
+      <c r="B21" s="5"/>
       <c r="G21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H21" s="3">
         <v>8</v>
@@ -988,26 +1159,32 @@
         <v>9</v>
       </c>
       <c r="J21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="B22" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -1015,40 +1192,40 @@
         <v>27</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1060,138 +1237,174 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="6:15">
       <c r="I59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L59" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="6:15">
       <c r="I60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="6:15">
       <c r="I61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="6:15">
       <c r="I62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L62" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="6:15">
       <c r="F63" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H63">
         <v>5</v>
       </c>
       <c r="I63" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O63">
         <v>5</v>
@@ -1199,31 +1412,31 @@
     </row>
     <row r="64" spans="6:15">
       <c r="F64" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H64">
         <v>5</v>
       </c>
       <c r="I64" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L64" t="s">
+        <v>73</v>
+      </c>
+      <c r="M64" t="s">
         <v>74</v>
       </c>
-      <c r="M64" t="s">
-        <v>75</v>
-      </c>
       <c r="N64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O64">
         <v>5</v>
@@ -1231,31 +1444,31 @@
     </row>
     <row r="65" spans="6:15">
       <c r="F65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H65">
         <v>5</v>
       </c>
       <c r="I65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O65">
         <v>5</v>
@@ -1263,31 +1476,31 @@
     </row>
     <row r="66" spans="6:15">
       <c r="F66" t="s">
+        <v>76</v>
+      </c>
+      <c r="G66" t="s">
         <v>77</v>
-      </c>
-      <c r="G66" t="s">
-        <v>78</v>
       </c>
       <c r="H66">
         <v>5</v>
       </c>
       <c r="I66" t="s">
+        <v>76</v>
+      </c>
+      <c r="J66" t="s">
+        <v>78</v>
+      </c>
+      <c r="K66" t="s">
+        <v>78</v>
+      </c>
+      <c r="L66" t="s">
+        <v>87</v>
+      </c>
+      <c r="M66" t="s">
+        <v>86</v>
+      </c>
+      <c r="N66" t="s">
         <v>77</v>
-      </c>
-      <c r="J66" t="s">
-        <v>79</v>
-      </c>
-      <c r="K66" t="s">
-        <v>79</v>
-      </c>
-      <c r="L66" t="s">
-        <v>88</v>
-      </c>
-      <c r="M66" t="s">
-        <v>87</v>
-      </c>
-      <c r="N66" t="s">
-        <v>78</v>
       </c>
       <c r="O66">
         <v>5</v>
@@ -1295,6 +1508,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>